<commit_message>
Info sheet and pooling script
</commit_message>
<xml_diff>
--- a/EUConnect19/data/admin/CourseInfo.xlsx
+++ b/EUConnect19/data/admin/CourseInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\LinkedDataWorkshop\EUConnect19\data\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20477020-95DD-467F-94B2-4223EBB25A41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC0A8CB-C1BC-4EE0-AA8F-D1C787F9A13F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13670" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Servers" sheetId="2" r:id="rId1"/>
@@ -65,8 +65,42 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Williams Tim</author>
+  </authors>
+  <commentList>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{BDAE64F1-47F6-4B12-9C0A-8A57CE5EFB77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Williams Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Includes start of Graph Editor</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="89">
   <si>
     <t>Comment</t>
   </si>
@@ -304,7 +338,67 @@
     <t>Studio Version</t>
   </si>
   <si>
-    <t>Studio shows correct shortcuts, files, databaseses</t>
+    <t>As phuseldw: Studio shows correct shortcuts, files, databaseses</t>
+  </si>
+  <si>
+    <t>Disable Java update</t>
+  </si>
+  <si>
+    <t>Study in Test loaded</t>
+  </si>
+  <si>
+    <t>AllStudies Merge Test</t>
+  </si>
+  <si>
+    <t>54.148.147.180</t>
+  </si>
+  <si>
+    <t>35.167.252.62</t>
+  </si>
+  <si>
+    <t>54.200.43.255</t>
+  </si>
+  <si>
+    <t>18.237.225.108</t>
+  </si>
+  <si>
+    <t>35.162.217.55</t>
+  </si>
+  <si>
+    <t>54.202.54.138</t>
+  </si>
+  <si>
+    <t>34.211.58.197</t>
+  </si>
+  <si>
+    <t>54.245.52.99</t>
+  </si>
+  <si>
+    <t>54.200.183.88</t>
+  </si>
+  <si>
+    <t>18.237.137.64</t>
+  </si>
+  <si>
+    <t>18.237.43.88</t>
+  </si>
+  <si>
+    <t>18.237.62.27</t>
+  </si>
+  <si>
+    <t>MASTER</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>phuseldw password reset</t>
+  </si>
+  <si>
+    <t>R  pkgs: DT, rdflib</t>
+  </si>
+  <si>
+    <t>Stardog Studio Version</t>
   </si>
 </sst>
 </file>
@@ -391,7 +485,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,19 +506,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,7 +523,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -500,17 +582,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -525,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -540,9 +611,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -567,9 +635,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,9 +646,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -594,11 +656,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -607,66 +668,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -675,7 +723,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -684,10 +732,34 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1009,928 +1081,1073 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="6.54296875" style="20" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="7.81640625" style="20" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="6.54296875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" style="18" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.54296875" style="20" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.54296875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="11" style="20" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" style="20" customWidth="1"/>
-    <col min="15" max="15" width="15.54296875" customWidth="1"/>
-    <col min="16" max="16" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="67.453125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="37.81640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="23.54296875" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" customWidth="1"/>
+    <col min="9" max="14" width="12.54296875" style="18" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="10.54296875" style="18" customWidth="1"/>
+    <col min="18" max="18" width="11" style="18" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" style="18" customWidth="1"/>
+    <col min="20" max="20" width="15.54296875" customWidth="1"/>
+    <col min="21" max="21" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="67.453125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="37.81640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="23.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="60" t="s">
+      <c r="H1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="L1" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="P1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="Q1" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="R1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="S1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="T1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="U1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="V1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="W1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="6"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="49">
-        <v>1</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="50" t="s">
+      <c r="X1" s="6"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" s="47">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="52" t="str">
+      <c r="D2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="7" t="str">
         <f>_xlfn.CONCAT("Study", A2)</f>
         <v>Study1</v>
       </c>
-      <c r="G2" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="61"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="S2" s="6"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="53">
-        <f t="shared" ref="A3:A21" si="0">A2+1</f>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="66"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="19"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="6"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3" s="47">
+        <f t="shared" ref="A3:A23" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15"/>
       <c r="F3" s="7" t="str">
-        <f>_xlfn.CONCAT("Study", A3)</f>
+        <f t="shared" ref="F3:F19" si="1">_xlfn.CONCAT("Study", A3)</f>
         <v>Study2</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="6"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="53">
+      <c r="G3" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="67"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="6"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" s="47">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15"/>
       <c r="F4" s="7" t="str">
-        <f t="shared" ref="F4:F20" si="1">_xlfn.CONCAT("Study", A4)</f>
+        <f t="shared" si="1"/>
         <v>Study3</v>
       </c>
-      <c r="G4" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="63"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="66"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
-      <c r="S4" s="6"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="53">
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="6"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A5" s="47">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="15"/>
       <c r="F5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study4</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="62"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="6"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="53">
+        <v>19</v>
+      </c>
+      <c r="H5" s="66"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="6"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A6" s="47">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="15"/>
       <c r="F6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study5</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="6"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="53">
+        <v>20</v>
+      </c>
+      <c r="H6" s="66"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="6"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A7" s="47">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="D7" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="15"/>
       <c r="F7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study6</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="62"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="6"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="53">
+        <v>21</v>
+      </c>
+      <c r="H7" s="66"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="6"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A8" s="47">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="D8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15"/>
       <c r="F8" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study7</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="62"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="6"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="53">
+        <v>22</v>
+      </c>
+      <c r="H8" s="66"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="6"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A9" s="47">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15"/>
       <c r="F9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study8</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="6"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="53">
+        <v>23</v>
+      </c>
+      <c r="H9" s="66"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="X9" s="6"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A10" s="47">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15"/>
       <c r="F10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study9</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="S10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="53">
+        <v>24</v>
+      </c>
+      <c r="H10" s="66"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="6"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A11" s="47">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="17"/>
       <c r="F11" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study10</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="H11" s="66"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="19"/>
       <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="6"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="53">
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="X11" s="6"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A12" s="47">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="17"/>
       <c r="F12" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study11</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="H12" s="66"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="19"/>
       <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="S12" s="6"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="53">
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="6"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A13" s="47">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="17"/>
       <c r="F13" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study12</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
+        <v>27</v>
+      </c>
+      <c r="H13" s="66"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="19"/>
       <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="6"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="53">
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="6"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A14" s="47">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="18"/>
+      <c r="D14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17"/>
       <c r="F14" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study13</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="H14" s="66"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="19"/>
       <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="6"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="53">
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="6"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A15" s="47">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="18"/>
+      <c r="D15" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="17"/>
       <c r="F15" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study14</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
+        <v>29</v>
+      </c>
+      <c r="H15" s="66"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="19"/>
       <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="6"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="53">
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="6"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A16" s="47">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="18"/>
+      <c r="D16" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="17"/>
       <c r="F16" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study15</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
+        <v>30</v>
+      </c>
+      <c r="H16" s="66"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="19"/>
       <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="6"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A17" s="53">
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="6"/>
+    </row>
+    <row r="17" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="47">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="18"/>
+      <c r="D17" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="17"/>
       <c r="F17" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study16</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
+        <v>31</v>
+      </c>
+      <c r="H17" s="66"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="19"/>
       <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="6"/>
-    </row>
-    <row r="18" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="53">
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="X17" s="8"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A18" s="47">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="18"/>
+      <c r="D18" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="17"/>
       <c r="F18" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study17</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
+        <v>32</v>
+      </c>
+      <c r="H18" s="66"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="53"/>
+      <c r="O18" s="19"/>
       <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="S18" s="9"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A19" s="54">
+      <c r="Q18" s="14"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="8"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A19" s="47">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="18"/>
+      <c r="D19" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="17"/>
       <c r="F19" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Study18</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="9"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A20" s="54">
+        <v>33</v>
+      </c>
+      <c r="H19" s="66"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="9"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A20" s="47">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="25"/>
+      <c r="B20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="17"/>
       <c r="F20" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("Study", A20)</f>
         <v>Study19</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S20" s="9"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="10"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A21" s="53">
+      <c r="G20" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="68"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="28"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="9"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A21" s="47">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="7" t="str">
+      <c r="B21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="27" t="str">
         <f>_xlfn.CONCAT("Study", A21)</f>
         <v>Study20</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="10"/>
-    </row>
-    <row r="22" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="53">
+      <c r="G21" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="V21" s="23"/>
+      <c r="W21" s="37"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="9"/>
+    </row>
+    <row r="22" spans="1:27" s="57" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="59">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="56"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="31" t="str">
+      <c r="B22" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="39"/>
+      <c r="F22" s="60" t="str">
         <f>_xlfn.CONCAT("Study", A22)</f>
         <v>Study21</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="58"/>
-      <c r="N22" s="59"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="59" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="43"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="10"/>
-    </row>
-    <row r="23" spans="1:22" s="27" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="41">
+      <c r="G22" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="56"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="56"/>
+      <c r="U22" s="56"/>
+      <c r="V22" s="56"/>
+      <c r="W22" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z22" s="58"/>
+    </row>
+    <row r="23" spans="1:27" s="24" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="59">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="35" t="s">
+      <c r="B23" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="39"/>
+      <c r="F23" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="42" t="s">
+      <c r="G23" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" s="56"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="56"/>
+      <c r="U23" s="56"/>
+      <c r="V23" s="56"/>
+      <c r="W23" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="U23" s="28"/>
-    </row>
-    <row r="24" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="G24" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="R24" s="28"/>
-      <c r="U24" s="28"/>
-    </row>
-    <row r="25" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="R25" s="28"/>
-      <c r="U25" s="28"/>
-    </row>
-    <row r="26" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
-      <c r="R26" s="28"/>
-      <c r="U26" s="28"/>
-    </row>
-    <row r="27" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="R27" s="28"/>
-      <c r="U27" s="28"/>
+      <c r="Z23" s="25"/>
+    </row>
+    <row r="24" spans="1:27" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="W24" s="25"/>
+      <c r="Z24" s="25"/>
+    </row>
+    <row r="25" spans="1:27" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="25"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="W25" s="25"/>
+      <c r="Z25" s="25"/>
+    </row>
+    <row r="26" spans="1:27" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="25"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="W26" s="25"/>
+      <c r="Z26" s="25"/>
     </row>
   </sheetData>
-  <sortState ref="B3:B12">
-    <sortCondition ref="B3:B12"/>
+  <sortState ref="B3:B23">
+    <sortCondition ref="B2:B23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1943,7 +2160,7 @@
   <dimension ref="B1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1964,7 +2181,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>43406</v>
       </c>
     </row>
@@ -1972,49 +2189,49 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C5" s="13"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C6" s="13"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C7" s="13"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C8" s="13"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C9" s="13"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C10" s="13"/>
+      <c r="C10" s="12"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C11" s="13"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C12" s="13"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C13" s="13"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C14" s="13"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C15" s="13"/>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C16" s="13"/>
+      <c r="C16" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2023,33 +2240,148 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CADFA43-8D08-4532-9E1D-2EE3C27FE678}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CADFA43-8D08-4532-9E1D-2EE3C27FE678}">
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="D1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="34" t="s">
         <v>51</v>
       </c>
     </row>
+    <row r="5" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="V5" s="6"/>
+      <c r="X5" s="1"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="38"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="V6" s="6"/>
+      <c r="X6" s="1"/>
+    </row>
   </sheetData>
+  <sortState ref="H1:H23">
+    <sortCondition ref="H1:H23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test data and config
</commit_message>
<xml_diff>
--- a/EUConnect19/data/admin/CourseInfo.xlsx
+++ b/EUConnect19/data/admin/CourseInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\LinkedDataWorkshop\EUConnect19\data\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC0A8CB-C1BC-4EE0-AA8F-D1C787F9A13F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CCBB32-B91A-448D-93E8-635DE1D5D50C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="91">
   <si>
     <t>Comment</t>
   </si>
@@ -278,9 +278,6 @@
     <t>C:\Users\phuseldw\AppData\Local\Programs\stardog-studio</t>
   </si>
   <si>
-    <t>KEEP</t>
-  </si>
-  <si>
     <t>NCT02049762</t>
   </si>
   <si>
@@ -392,13 +389,22 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>phuseldw password reset</t>
-  </si>
-  <si>
     <t>R  pkgs: DT, rdflib</t>
   </si>
   <si>
     <t>Stardog Studio Version</t>
+  </si>
+  <si>
+    <t>NO!</t>
+  </si>
+  <si>
+    <t>Clear all broswer hist. Confirm blank Predicate</t>
+  </si>
+  <si>
+    <t>ADMIN: phuseldw password reset</t>
+  </si>
+  <si>
+    <t>Admin: New content from Git to student area</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -761,6 +767,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1081,11 +1090,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA26"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,20 +1107,20 @@
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.54296875" customWidth="1"/>
-    <col min="9" max="14" width="12.54296875" style="18" customWidth="1"/>
-    <col min="15" max="15" width="10.453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.54296875" style="18" customWidth="1"/>
-    <col min="18" max="18" width="11" style="18" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" style="18" customWidth="1"/>
-    <col min="20" max="20" width="15.54296875" customWidth="1"/>
-    <col min="21" max="21" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="67.453125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="37.81640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="23.54296875" customWidth="1"/>
+    <col min="9" max="17" width="12.54296875" style="18" customWidth="1"/>
+    <col min="18" max="18" width="10.453125" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.54296875" style="18" customWidth="1"/>
+    <col min="21" max="21" width="11" style="18" customWidth="1"/>
+    <col min="22" max="22" width="10.54296875" style="18" customWidth="1"/>
+    <col min="23" max="23" width="15.54296875" customWidth="1"/>
+    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="67.453125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="37.81640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="23.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="87" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>2</v>
       </c>
@@ -1134,61 +1143,67 @@
         <v>35</v>
       </c>
       <c r="H1" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="K1" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="51" t="s">
+      <c r="M1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="P1" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="Q1" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="O1" s="29" t="s">
+      <c r="R1" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="T1" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="S1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="X1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="Y1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="Z1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="X1" s="6"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="AA1" s="6"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="47">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="64" t="s">
         <v>5</v>
@@ -1208,33 +1223,36 @@
       <c r="I2" s="53"/>
       <c r="J2" s="53"/>
       <c r="K2" s="53"/>
-      <c r="L2" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="19"/>
+      <c r="S2" s="30"/>
       <c r="T2" s="14"/>
       <c r="U2" s="14"/>
       <c r="V2" s="14"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="6"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="6"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="47">
         <f t="shared" ref="A3:A23" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="64" t="s">
         <v>5</v>
@@ -1257,24 +1275,27 @@
       <c r="L3" s="54"/>
       <c r="M3" s="54"/>
       <c r="N3" s="54"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="30"/>
       <c r="T3" s="14"/>
       <c r="U3" s="14"/>
       <c r="V3" s="14"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="6"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="6"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="47">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="64" t="s">
         <v>5</v>
@@ -1297,24 +1318,27 @@
       <c r="L4" s="53"/>
       <c r="M4" s="53"/>
       <c r="N4" s="53"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="30"/>
       <c r="T4" s="14"/>
       <c r="U4" s="14"/>
       <c r="V4" s="14"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="6"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="6"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="47">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="64" t="s">
         <v>5</v>
@@ -1337,24 +1361,27 @@
       <c r="L5" s="53"/>
       <c r="M5" s="53"/>
       <c r="N5" s="53"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="30"/>
       <c r="T5" s="14"/>
       <c r="U5" s="14"/>
       <c r="V5" s="14"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="6"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="6"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="47">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="64" t="s">
         <v>5</v>
@@ -1377,24 +1404,27 @@
       <c r="L6" s="53"/>
       <c r="M6" s="53"/>
       <c r="N6" s="53"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="30"/>
       <c r="T6" s="14"/>
       <c r="U6" s="14"/>
       <c r="V6" s="14"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="6"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="6"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="47">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="64" t="s">
         <v>5</v>
@@ -1417,24 +1447,27 @@
       <c r="L7" s="53"/>
       <c r="M7" s="53"/>
       <c r="N7" s="53"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="53"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="30"/>
       <c r="T7" s="14"/>
       <c r="U7" s="14"/>
       <c r="V7" s="14"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="6"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="6"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="47">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="64" t="s">
         <v>5</v>
@@ -1457,24 +1490,27 @@
       <c r="L8" s="53"/>
       <c r="M8" s="53"/>
       <c r="N8" s="53"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="30"/>
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
       <c r="V8" s="14"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="6"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="6"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="47">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="64" t="s">
         <v>5</v>
@@ -1497,23 +1533,26 @@
       <c r="L9" s="53"/>
       <c r="M9" s="53"/>
       <c r="N9" s="53"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="53"/>
+      <c r="Q9" s="53"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="30"/>
       <c r="T9" s="14"/>
       <c r="U9" s="14"/>
       <c r="V9" s="14"/>
-      <c r="X9" s="6"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="AA9" s="6"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="47">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="64" t="s">
         <v>5</v>
@@ -1536,24 +1575,27 @@
       <c r="L10" s="53"/>
       <c r="M10" s="53"/>
       <c r="N10" s="53"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="14"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="53"/>
+      <c r="Q10" s="53"/>
       <c r="R10" s="19"/>
-      <c r="S10" s="14"/>
+      <c r="S10" s="30"/>
       <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
+      <c r="U10" s="19"/>
       <c r="V10" s="14"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="6"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="6"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="47">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="64" t="s">
         <v>5</v>
@@ -1576,26 +1618,29 @@
       <c r="L11" s="53"/>
       <c r="M11" s="53"/>
       <c r="N11" s="53"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="53"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="15"/>
       <c r="T11" s="14"/>
       <c r="U11" s="14"/>
       <c r="V11" s="14"/>
-      <c r="W11" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="X11" s="6"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA11" s="6"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="47">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="64" t="s">
         <v>5</v>
@@ -1618,24 +1663,27 @@
       <c r="L12" s="53"/>
       <c r="M12" s="53"/>
       <c r="N12" s="53"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="53"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="15"/>
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="6"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="6"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="47">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="64" t="s">
         <v>5</v>
@@ -1658,24 +1706,27 @@
       <c r="L13" s="53"/>
       <c r="M13" s="53"/>
       <c r="N13" s="53"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="53"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="15"/>
       <c r="T13" s="14"/>
       <c r="U13" s="14"/>
       <c r="V13" s="14"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="6"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="6"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="47">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="64" t="s">
         <v>5</v>
@@ -1698,24 +1749,27 @@
       <c r="L14" s="53"/>
       <c r="M14" s="53"/>
       <c r="N14" s="53"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="53"/>
+      <c r="Q14" s="53"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="15"/>
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
       <c r="V14" s="14"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="6"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="47">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="64" t="s">
         <v>5</v>
@@ -1738,24 +1792,27 @@
       <c r="L15" s="53"/>
       <c r="M15" s="53"/>
       <c r="N15" s="53"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="53"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="15"/>
       <c r="T15" s="14"/>
       <c r="U15" s="14"/>
       <c r="V15" s="14"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="6"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="6"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" s="47">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="64" t="s">
         <v>5</v>
@@ -1778,24 +1835,27 @@
       <c r="L16" s="53"/>
       <c r="M16" s="53"/>
       <c r="N16" s="53"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="15"/>
       <c r="T16" s="14"/>
       <c r="U16" s="14"/>
       <c r="V16" s="14"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="6"/>
-    </row>
-    <row r="17" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="6"/>
+    </row>
+    <row r="17" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="47">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="64" t="s">
         <v>5</v>
@@ -1818,26 +1878,29 @@
       <c r="L17" s="53"/>
       <c r="M17" s="53"/>
       <c r="N17" s="53"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="15"/>
       <c r="T17" s="14"/>
       <c r="U17" s="14"/>
       <c r="V17" s="14"/>
-      <c r="W17" s="13" t="s">
+      <c r="W17" s="14"/>
+      <c r="X17" s="14"/>
+      <c r="Y17" s="14"/>
+      <c r="Z17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="X17" s="8"/>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AA17" s="8"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A18" s="47">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="64" t="s">
         <v>5</v>
@@ -1860,24 +1923,27 @@
       <c r="L18" s="53"/>
       <c r="M18" s="53"/>
       <c r="N18" s="53"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="14"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="53"/>
       <c r="R18" s="19"/>
-      <c r="S18" s="14"/>
+      <c r="S18" s="15"/>
       <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
+      <c r="U18" s="19"/>
       <c r="V18" s="14"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="8"/>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="8"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A19" s="47">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="64" t="s">
         <v>5</v>
@@ -1900,29 +1966,32 @@
       <c r="L19" s="53"/>
       <c r="M19" s="53"/>
       <c r="N19" s="53"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="14"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="53"/>
       <c r="R19" s="19"/>
-      <c r="S19" s="14"/>
+      <c r="S19" s="23"/>
       <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
+      <c r="U19" s="19"/>
       <c r="V19" s="14"/>
-      <c r="W19" s="28" t="s">
+      <c r="W19" s="14"/>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="10"/>
-      <c r="AA19" s="9"/>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="9"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A20" s="47">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="64" t="s">
         <v>5</v>
@@ -1945,27 +2014,30 @@
       <c r="L20" s="53"/>
       <c r="M20" s="53"/>
       <c r="N20" s="53"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="14"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="53"/>
       <c r="R20" s="19"/>
-      <c r="S20" s="14"/>
+      <c r="S20" s="23"/>
       <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
+      <c r="U20" s="19"/>
       <c r="V20" s="14"/>
-      <c r="W20" s="28"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="10"/>
-      <c r="AA20" s="9"/>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="28"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="9"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A21" s="47">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="64" t="s">
         <v>5</v>
@@ -1984,37 +2056,36 @@
       <c r="H21" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="I21" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="J21" s="55" t="s">
+      <c r="I21" s="55"/>
+      <c r="J21" s="70" t="s">
         <v>1</v>
       </c>
       <c r="K21" s="55"/>
       <c r="L21" s="55"/>
       <c r="M21" s="55"/>
       <c r="N21" s="55"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="50"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
       <c r="R21" s="49"/>
-      <c r="S21" s="50"/>
+      <c r="S21" s="23"/>
       <c r="T21" s="50"/>
-      <c r="U21" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="V21" s="23"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="9"/>
-    </row>
-    <row r="22" spans="1:27" s="57" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="59">
+      <c r="U21" s="49"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="37"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="9"/>
+    </row>
+    <row r="22" spans="1:30" s="57" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="71">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="65" t="s">
         <v>7</v>
@@ -2028,35 +2099,52 @@
         <v>Study21</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="56"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
+        <v>48</v>
+      </c>
+      <c r="H22" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="17" t="s">
+        <v>1</v>
+      </c>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
+      <c r="R22" s="17" t="s">
+        <v>1</v>
+      </c>
       <c r="S22" s="17"/>
-      <c r="T22" s="56"/>
-      <c r="U22" s="56"/>
-      <c r="V22" s="56"/>
-      <c r="W22" s="61" t="s">
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="56"/>
+      <c r="X22" s="56"/>
+      <c r="Y22" s="56"/>
+      <c r="Z22" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="Z22" s="58"/>
-    </row>
-    <row r="23" spans="1:27" s="24" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="AC22" s="58"/>
+    </row>
+    <row r="23" spans="1:30" s="24" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="59">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="48" t="s">
         <v>36</v>
@@ -2069,7 +2157,7 @@
         <v>39</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H23" s="56"/>
       <c r="I23" s="17"/>
@@ -2083,15 +2171,20 @@
       <c r="Q23" s="17"/>
       <c r="R23" s="17"/>
       <c r="S23" s="17"/>
-      <c r="T23" s="56"/>
-      <c r="U23" s="56"/>
-      <c r="V23" s="56"/>
-      <c r="W23" s="59" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z23" s="25"/>
-    </row>
-    <row r="24" spans="1:27" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="56"/>
+      <c r="X23" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y23" s="56"/>
+      <c r="Z23" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC23" s="25"/>
+    </row>
+    <row r="24" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="25"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
@@ -2106,10 +2199,13 @@
       <c r="Q24" s="26"/>
       <c r="R24" s="26"/>
       <c r="S24" s="26"/>
-      <c r="W24" s="25"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
       <c r="Z24" s="25"/>
-    </row>
-    <row r="25" spans="1:27" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="AC24" s="25"/>
+    </row>
+    <row r="25" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="25"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
@@ -2124,10 +2220,13 @@
       <c r="Q25" s="26"/>
       <c r="R25" s="26"/>
       <c r="S25" s="26"/>
-      <c r="W25" s="25"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="26"/>
+      <c r="V25" s="26"/>
       <c r="Z25" s="25"/>
-    </row>
-    <row r="26" spans="1:27" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="AC25" s="25"/>
+    </row>
+    <row r="26" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="25"/>
       <c r="D26" s="26"/>
       <c r="E26" s="26"/>
@@ -2142,8 +2241,11 @@
       <c r="Q26" s="26"/>
       <c r="R26" s="26"/>
       <c r="S26" s="26"/>
-      <c r="W26" s="25"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
       <c r="Z26" s="25"/>
+      <c r="AC26" s="25"/>
     </row>
   </sheetData>
   <sortState ref="B3:B23">
@@ -2255,15 +2357,15 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="D1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="87" x14ac:dyDescent="0.35">
@@ -2289,19 +2391,19 @@
         <v>35</v>
       </c>
       <c r="H5" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="51" t="s">
+      <c r="J5" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="J5" s="51" t="s">
+      <c r="K5" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="K5" s="51" t="s">
+      <c r="L5" s="51" t="s">
         <v>70</v>
-      </c>
-      <c r="L5" s="51" t="s">
-        <v>71</v>
       </c>
       <c r="M5" s="29" t="s">
         <v>41</v>
@@ -2335,21 +2437,21 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="45"/>
       <c r="E6" s="45"/>
       <c r="F6" s="46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="52"/>
       <c r="I6" s="52"/>
@@ -2371,7 +2473,7 @@
       <c r="S6" s="40"/>
       <c r="T6" s="40"/>
       <c r="U6" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="V6" s="6"/>
       <c r="X6" s="1"/>

</xml_diff>

<commit_message>
Added correct NCT id to test studyies
</commit_message>
<xml_diff>
--- a/EUConnect19/data/admin/CourseInfo.xlsx
+++ b/EUConnect19/data/admin/CourseInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\LinkedDataWorkshop\EUConnect19\data\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C672A26B-748F-4484-BB6A-5E746C3BB4EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1D3119-7286-4C3D-B735-468FBD373499}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="102">
   <si>
     <t>Comment</t>
   </si>
@@ -466,9 +466,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Correct SD STudio Shortcut</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -478,10 +475,19 @@
     <t>not checked</t>
   </si>
   <si>
-    <t>Only file in C:\LInkedDataWorkshop\Data  is StudyOntology.TTL  (DEL .JSON and Whitboard file.)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> /Downloads is empty</t>
+  </si>
+  <si>
+    <t>Only file in C:\LinkedDataWorkshop\Data  is StudyOntology.TTL  (DEL .JSON and Whitboard file.)</t>
+  </si>
+  <si>
+    <t>NotePad++: No files open, updating disabled</t>
+  </si>
+  <si>
+    <t>not confirmed</t>
+  </si>
+  <si>
+    <t>Correct SD Studio Shortcut</t>
   </si>
 </sst>
 </file>
@@ -691,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -832,9 +838,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -844,9 +847,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -860,12 +860,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -878,7 +872,16 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1200,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1215,19 +1218,21 @@
     <col min="4" max="4" width="6.54296875" style="18" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="17" width="12.54296875" style="18" customWidth="1"/>
-    <col min="18" max="18" width="12.54296875" style="74" customWidth="1"/>
-    <col min="19" max="19" width="12.54296875" style="18" customWidth="1"/>
-    <col min="20" max="20" width="10.54296875" style="18" customWidth="1"/>
-    <col min="21" max="21" width="15.54296875" customWidth="1"/>
-    <col min="22" max="22" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="67.453125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="37.81640625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="23.54296875" customWidth="1"/>
+    <col min="7" max="8" width="12.54296875" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" style="70" customWidth="1"/>
+    <col min="10" max="18" width="12.54296875" style="18" customWidth="1"/>
+    <col min="19" max="19" width="18" style="18" customWidth="1"/>
+    <col min="21" max="21" width="12.54296875" style="18" customWidth="1"/>
+    <col min="22" max="22" width="10.54296875" style="18" customWidth="1"/>
+    <col min="23" max="23" width="15.54296875" customWidth="1"/>
+    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="67.453125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="37.81640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="23.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
         <v>2</v>
       </c>
@@ -1246,70 +1251,73 @@
       <c r="F1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="K1" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="L1" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="75" t="s">
-        <v>94</v>
-      </c>
-      <c r="M1" s="75" t="s">
+      <c r="M1" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="75" t="s">
-        <v>96</v>
-      </c>
-      <c r="O1" s="75" t="s">
+      <c r="O1" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="P1" s="75" t="s">
+      <c r="Q1" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="75" t="s">
+      <c r="R1" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="S1" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="R1" s="70" t="s">
-        <v>98</v>
-      </c>
-      <c r="S1" s="49" t="s">
+      <c r="U1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="X1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="Y1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="Z1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="Y1" s="6"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA1" s="6"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="46">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="15" t="s">
@@ -1322,37 +1330,64 @@
       <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="29"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
+      <c r="G2" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="29"/>
       <c r="W2" s="14"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="6"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="6"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="46">
         <f t="shared" ref="A3:A23" si="0">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="15" t="s">
@@ -1365,35 +1400,62 @@
       <c r="F3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
+      <c r="G3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" s="52"/>
+      <c r="V3" s="29"/>
       <c r="W3" s="14"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="6"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="46">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -1406,35 +1468,62 @@
       <c r="F4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
+      <c r="G4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" s="51"/>
+      <c r="V4" s="29"/>
       <c r="W4" s="14"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="6"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="46">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1447,35 +1536,62 @@
       <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
+      <c r="G5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" s="51"/>
+      <c r="V5" s="29"/>
       <c r="W5" s="14"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="6"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="6"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="46">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="15" t="s">
@@ -1488,35 +1604,62 @@
       <c r="F6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="51"/>
-      <c r="R6" s="51"/>
-      <c r="S6" s="51"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
+      <c r="G6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U6" s="51"/>
+      <c r="V6" s="29"/>
       <c r="W6" s="14"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="6"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="46">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="15" t="s">
@@ -1529,35 +1672,62 @@
       <c r="F7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="51"/>
-      <c r="S7" s="51"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
+      <c r="G7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7" s="51"/>
+      <c r="V7" s="29"/>
       <c r="W7" s="14"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="6"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="6"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="46">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -1570,35 +1740,62 @@
       <c r="F8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
+      <c r="G8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="51"/>
+      <c r="V8" s="29"/>
       <c r="W8" s="14"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="6"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="6"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="46">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="15" t="s">
@@ -1611,34 +1808,61 @@
       <c r="F9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="51"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
+      <c r="G9" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" s="51"/>
+      <c r="V9" s="29"/>
       <c r="W9" s="14"/>
-      <c r="Y9" s="6"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="AA9" s="6"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="46">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -1651,35 +1875,62 @@
       <c r="F10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="51"/>
-      <c r="R10" s="51"/>
-      <c r="S10" s="51"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
+      <c r="G10" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10" s="51"/>
+      <c r="V10" s="29"/>
       <c r="W10" s="14"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="6"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="6"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="46">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="15" t="s">
@@ -1692,37 +1943,64 @@
       <c r="F11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="51"/>
-      <c r="S11" s="51"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
+      <c r="G11" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S11" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U11" s="51"/>
+      <c r="V11" s="15"/>
       <c r="W11" s="14"/>
-      <c r="X11" s="11" t="s">
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="Y11" s="6"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA11" s="6"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="46">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1735,27 +2013,54 @@
       <c r="F12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="51"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
+      <c r="G12" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P12" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S12" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U12" s="51"/>
+      <c r="V12" s="15"/>
       <c r="W12" s="14"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="6"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="6"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="46">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1763,7 +2068,7 @@
       <c r="B13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -1776,35 +2081,44 @@
       <c r="F13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
+      <c r="G13" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="51" t="s">
+        <v>1</v>
+      </c>
       <c r="M13" s="51"/>
       <c r="N13" s="51"/>
       <c r="O13" s="51"/>
       <c r="P13" s="51"/>
       <c r="Q13" s="51"/>
       <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
+      <c r="S13" s="29"/>
+      <c r="U13" s="51"/>
+      <c r="V13" s="15"/>
       <c r="W13" s="14"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="6"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="6"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="46">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="62" t="s">
+      <c r="C14" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="15" t="s">
@@ -1817,35 +2131,62 @@
       <c r="F14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="51"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
+      <c r="G14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" s="51"/>
+      <c r="V14" s="15"/>
       <c r="W14" s="14"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="6"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="46">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="15" t="s">
@@ -1858,35 +2199,62 @@
       <c r="F15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="51"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
+      <c r="G15" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="K15" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="L15" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="M15" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S15" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U15" s="51"/>
+      <c r="V15" s="15"/>
       <c r="W15" s="14"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="6"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="6"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" s="46">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="15" t="s">
@@ -1899,35 +2267,62 @@
       <c r="F16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="51"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
+      <c r="G16" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S16" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U16" s="51"/>
+      <c r="V16" s="15"/>
       <c r="W16" s="14"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="6"/>
-    </row>
-    <row r="17" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="6"/>
+    </row>
+    <row r="17" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="46">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="15" t="s">
@@ -1940,37 +2335,64 @@
       <c r="F17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="51"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
+      <c r="G17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="U17" s="51"/>
+      <c r="V17" s="15"/>
       <c r="W17" s="14"/>
-      <c r="X17" s="13" t="s">
+      <c r="X17" s="14"/>
+      <c r="Y17" s="14"/>
+      <c r="Z17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="Y17" s="8"/>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AA17" s="8"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A18" s="46">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="15" t="s">
@@ -1986,18 +2408,20 @@
       <c r="G18" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="51"/>
+      <c r="H18" s="51" t="s">
+        <v>1</v>
+      </c>
       <c r="I18" s="51" t="s">
         <v>1</v>
       </c>
       <c r="J18" s="51" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="K18" s="51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L18" s="51" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="M18" s="51" t="s">
         <v>1</v>
@@ -2006,10 +2430,10 @@
         <v>1</v>
       </c>
       <c r="O18" s="51" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="P18" s="51" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="Q18" s="51" t="s">
         <v>1</v>
@@ -2017,23 +2441,26 @@
       <c r="R18" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="S18" s="51"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
+      <c r="S18" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="U18" s="51"/>
+      <c r="V18" s="15"/>
       <c r="W18" s="14"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="8"/>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="8"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A19" s="46">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="15" t="s">
@@ -2068,10 +2495,10 @@
         <v>1</v>
       </c>
       <c r="N19" s="51" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="O19" s="51" t="s">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="P19" s="51" t="s">
         <v>1</v>
@@ -2079,29 +2506,34 @@
       <c r="Q19" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="R19" s="71"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="22"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
+      <c r="R19" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S19" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="U19" s="51"/>
+      <c r="V19" s="22"/>
       <c r="W19" s="14"/>
-      <c r="X19" s="27" t="s">
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="10"/>
+      <c r="AA19" s="8"/>
       <c r="AB19" s="9"/>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="9"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A20" s="46">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="62" t="s">
+      <c r="C20" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="15" t="s">
@@ -2111,10 +2543,10 @@
         <f>_xlfn.CONCAT("Study", A20)</f>
         <v>Study19</v>
       </c>
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="67" t="s">
+      <c r="G20" s="65" t="s">
         <v>1</v>
       </c>
       <c r="H20" s="51" t="s">
@@ -2136,10 +2568,10 @@
         <v>1</v>
       </c>
       <c r="N20" s="51" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="O20" s="51" t="s">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="P20" s="51" t="s">
         <v>1</v>
@@ -2147,27 +2579,32 @@
       <c r="Q20" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="R20" s="71"/>
-      <c r="S20" s="51"/>
-      <c r="T20" s="22"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
+      <c r="R20" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="S20" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="U20" s="51"/>
+      <c r="V20" s="22"/>
       <c r="W20" s="14"/>
-      <c r="X20" s="27"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="10"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="8"/>
       <c r="AB20" s="9"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="9"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A21" s="46">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="62" t="s">
+      <c r="C21" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="15" t="s">
@@ -2183,13 +2620,13 @@
       <c r="G21" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="J21" s="53" t="s">
+      <c r="H21" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="63" t="s">
         <v>1</v>
       </c>
       <c r="K21" s="53" t="s">
@@ -2201,11 +2638,11 @@
       <c r="M21" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="N21" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="O21" s="53" t="s">
-        <v>1</v>
+      <c r="N21" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" s="51" t="s">
+        <v>96</v>
       </c>
       <c r="P21" s="53" t="s">
         <v>1</v>
@@ -2213,44 +2650,49 @@
       <c r="Q21" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="R21" s="64"/>
-      <c r="S21" s="53"/>
-      <c r="T21" s="22"/>
-      <c r="U21" s="48"/>
-      <c r="V21" s="48"/>
-      <c r="W21" s="22"/>
-      <c r="X21" s="36"/>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="9"/>
-    </row>
-    <row r="22" spans="1:28" s="55" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="66">
+      <c r="R21" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="S21" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="U21" s="53"/>
+      <c r="V21" s="22"/>
+      <c r="W21" s="48"/>
+      <c r="X21" s="48"/>
+      <c r="Y21" s="22"/>
+      <c r="Z21" s="36"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="9"/>
+    </row>
+    <row r="22" spans="1:30" s="55" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="64">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="63" t="s">
+      <c r="C22" s="62" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="58" t="str">
+      <c r="E22" s="74" t="str">
         <f>_xlfn.CONCAT("Study", A22)</f>
         <v>Study21</v>
       </c>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="62" t="s">
         <v>48</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I22" s="17" t="s">
+      <c r="H22" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="51" t="s">
         <v>1</v>
       </c>
       <c r="J22" s="17" t="s">
@@ -2265,11 +2707,11 @@
       <c r="M22" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="N22" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="O22" s="17" t="s">
-        <v>1</v>
+      <c r="N22" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O22" s="51" t="s">
+        <v>96</v>
       </c>
       <c r="P22" s="17" t="s">
         <v>1</v>
@@ -2277,18 +2719,23 @@
       <c r="Q22" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="R22" s="76"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="54"/>
-      <c r="V22" s="54"/>
+      <c r="R22" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="S22" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
       <c r="W22" s="54"/>
-      <c r="X22" s="59" t="s">
+      <c r="X22" s="54"/>
+      <c r="Y22" s="54"/>
+      <c r="Z22" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="AA22" s="56"/>
-    </row>
-    <row r="23" spans="1:28" s="23" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="AC22" s="56"/>
+    </row>
+    <row r="23" spans="1:30" s="23" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="57">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2302,7 +2749,7 @@
       <c r="D23" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="59" t="s">
         <v>39</v>
       </c>
       <c r="F23" s="34" t="s">
@@ -2310,7 +2757,7 @@
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
+      <c r="I23" s="68"/>
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
@@ -2320,24 +2767,25 @@
       <c r="P23" s="17"/>
       <c r="Q23" s="17"/>
       <c r="R23" s="72"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="54" t="s">
+      <c r="S23" s="29"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="54"/>
+      <c r="X23" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="W23" s="54"/>
-      <c r="X23" s="57" t="s">
+      <c r="Y23" s="54"/>
+      <c r="Z23" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="AA23" s="24"/>
-    </row>
-    <row r="24" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="AC23" s="24"/>
+    </row>
+    <row r="24" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
       <c r="D24" s="25"/>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
+      <c r="I24" s="69"/>
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
       <c r="L24" s="25"/>
@@ -2346,18 +2794,19 @@
       <c r="O24" s="25"/>
       <c r="P24" s="25"/>
       <c r="Q24" s="25"/>
-      <c r="R24" s="73"/>
+      <c r="R24" s="25"/>
       <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
-      <c r="X24" s="24"/>
-      <c r="AA24" s="24"/>
-    </row>
-    <row r="25" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="Z24" s="24"/>
+      <c r="AC24" s="24"/>
+    </row>
+    <row r="25" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="D25" s="25"/>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
+      <c r="I25" s="69"/>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
       <c r="L25" s="25"/>
@@ -2366,18 +2815,19 @@
       <c r="O25" s="25"/>
       <c r="P25" s="25"/>
       <c r="Q25" s="25"/>
-      <c r="R25" s="73"/>
+      <c r="R25" s="25"/>
       <c r="S25" s="25"/>
-      <c r="T25" s="25"/>
-      <c r="X25" s="24"/>
-      <c r="AA25" s="24"/>
-    </row>
-    <row r="26" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="Z25" s="24"/>
+      <c r="AC25" s="24"/>
+    </row>
+    <row r="26" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="24"/>
       <c r="D26" s="25"/>
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
+      <c r="I26" s="69"/>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
       <c r="L26" s="25"/>
@@ -2386,11 +2836,12 @@
       <c r="O26" s="25"/>
       <c r="P26" s="25"/>
       <c r="Q26" s="25"/>
-      <c r="R26" s="73"/>
+      <c r="R26" s="25"/>
       <c r="S26" s="25"/>
-      <c r="T26" s="25"/>
-      <c r="X26" s="24"/>
-      <c r="AA26" s="24"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
+      <c r="Z26" s="24"/>
+      <c r="AC26" s="24"/>
     </row>
   </sheetData>
   <sortState ref="B3:B23">

</xml_diff>

<commit_message>
first working version. Label needs to be added
</commit_message>
<xml_diff>
--- a/EUConnect19/data/admin/CourseInfo.xlsx
+++ b/EUConnect19/data/admin/CourseInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\LinkedDataWorkshop\EUConnect19\data\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B435AE9-A5DA-4C61-B10B-3C3B98A890C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93361152-D8AB-4E0C-B3D2-DA96B52C57BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="106">
   <si>
     <t>Comment</t>
   </si>
@@ -497,6 +497,9 @@
   </si>
   <si>
     <t>NCT00474903</t>
+  </si>
+  <si>
+    <t>wants to update</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -644,8 +647,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -714,11 +723,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -915,7 +935,13 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1239,7 +1265,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1356,7 +1382,7 @@
       <c r="A2" s="43">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="78" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="58" t="s">
@@ -1435,7 +1461,7 @@
         <f t="shared" ref="A3:A23" si="0">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="78" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="58" t="s">
@@ -1512,7 +1538,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="78" t="s">
         <v>78</v>
       </c>
       <c r="C4" s="58" t="s">
@@ -1589,7 +1615,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="78" t="s">
         <v>72</v>
       </c>
       <c r="C5" s="58" t="s">
@@ -1602,7 +1628,7 @@
         <f t="shared" si="1"/>
         <v>Study4</v>
       </c>
-      <c r="F5" s="78" t="s">
+      <c r="F5" s="82" t="s">
         <v>103</v>
       </c>
       <c r="G5" s="48" t="s">
@@ -1666,7 +1692,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="78" t="s">
         <v>79</v>
       </c>
       <c r="C6" s="58" t="s">
@@ -1743,7 +1769,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="78" t="s">
         <v>80</v>
       </c>
       <c r="C7" s="58" t="s">
@@ -1820,7 +1846,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="78" t="s">
         <v>75</v>
       </c>
       <c r="C8" s="58" t="s">
@@ -1833,7 +1859,7 @@
         <f t="shared" si="1"/>
         <v>Study7</v>
       </c>
-      <c r="F8" s="78" t="s">
+      <c r="F8" s="82" t="s">
         <v>104</v>
       </c>
       <c r="G8" s="48" t="s">
@@ -1897,7 +1923,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="78" t="s">
         <v>61</v>
       </c>
       <c r="C9" s="58" t="s">
@@ -1973,7 +1999,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="78" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="58" t="s">
@@ -2050,7 +2076,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="78" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="58" t="s">
@@ -2129,7 +2155,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="78" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="58" t="s">
@@ -2206,7 +2232,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="78" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="58" t="s">
@@ -2283,7 +2309,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="78" t="s">
         <v>70</v>
       </c>
       <c r="C14" s="58" t="s">
@@ -2360,7 +2386,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="78" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="58" t="s">
@@ -2437,7 +2463,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="78" t="s">
         <v>56</v>
       </c>
       <c r="C16" s="58" t="s">
@@ -2514,7 +2540,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="78" t="s">
         <v>69</v>
       </c>
       <c r="C17" s="58" t="s">
@@ -2593,7 +2619,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="80" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="58" t="s">
@@ -2670,7 +2696,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="80" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="58" t="s">
@@ -2712,6 +2738,9 @@
       </c>
       <c r="O19" s="64" t="s">
         <v>1</v>
+      </c>
+      <c r="P19" s="81" t="s">
+        <v>105</v>
       </c>
       <c r="Q19" s="48" t="s">
         <v>1</v>
@@ -2752,7 +2781,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="78" t="s">
         <v>77</v>
       </c>
       <c r="C20" s="58" t="s">
@@ -2832,7 +2861,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="79" t="s">
         <v>71</v>
       </c>
       <c r="C21" s="74" t="s">
@@ -2910,7 +2939,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="78" t="s">
         <v>74</v>
       </c>
       <c r="C22" s="59" t="s">

</xml_diff>